<commit_message>
Revise audio controller board to use demultiplexers instead of relay
</commit_message>
<xml_diff>
--- a/electrical/AudioPassController-BOM.xlsx
+++ b/electrical/AudioPassController-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Random Files\programs and stuff taht I made\Automatic-Turntable\electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CA6C93-755C-45E6-A2EB-B29354426F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F696F952-6542-470D-B750-C453C05CFEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -31,17 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>Ceramic Capacitor</t>
   </si>
   <si>
-    <t>Rectifier Diode</t>
-  </si>
-  <si>
-    <t>Basic FET P-Channel</t>
-  </si>
-  <si>
     <t>Part Number</t>
   </si>
   <si>
@@ -54,9 +48,6 @@
     <t>Price Est.</t>
   </si>
   <si>
-    <t>TIP120</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -78,21 +69,12 @@
     <t>Value(s)</t>
   </si>
   <si>
-    <t>300 mil</t>
-  </si>
-  <si>
     <t>0603</t>
   </si>
   <si>
-    <t>1N4007</t>
-  </si>
-  <si>
     <t>Resistor</t>
   </si>
   <si>
-    <t>TO220</t>
-  </si>
-  <si>
     <t>Total (where applicable):</t>
   </si>
   <si>
@@ -102,48 +84,15 @@
     <t>0805</t>
   </si>
   <si>
-    <t>1kΩ; ±5%; 1/4w</t>
-  </si>
-  <si>
-    <t>ERJ-PA3J102V</t>
-  </si>
-  <si>
     <t>Substitute Part #</t>
   </si>
   <si>
     <t>--</t>
   </si>
   <si>
-    <t>Relay</t>
-  </si>
-  <si>
-    <t>J104D2C5VDC.20S</t>
-  </si>
-  <si>
-    <t>DPDT (2 Form C)</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
-    <t>1µF; 16V</t>
-  </si>
-  <si>
-    <t>0805YD105KAT2A</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>RL1</t>
-  </si>
-  <si>
     <t>male header - 3 pins (1 row)</t>
   </si>
   <si>
@@ -172,6 +121,60 @@
   </si>
   <si>
     <t>Price estimates are as of 2 Oct. 2022</t>
+  </si>
+  <si>
+    <t>10µF</t>
+  </si>
+  <si>
+    <t>CL21A106KOQNNNE</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>1µF</t>
+  </si>
+  <si>
+    <t>CL21B105KAFNNNE</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>47nF</t>
+  </si>
+  <si>
+    <t>C4, C5</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>CL21B104KACNNNC</t>
+  </si>
+  <si>
+    <t>10kΩ; ±5%; 1/4w</t>
+  </si>
+  <si>
+    <t>ERJ-PA3F1002V</t>
+  </si>
+  <si>
+    <t>R1, R2</t>
+  </si>
+  <si>
+    <t>U1, U2</t>
+  </si>
+  <si>
+    <t>1:2 demultiplexer</t>
+  </si>
+  <si>
+    <t>SN74LVC1G18DBVR</t>
+  </si>
+  <si>
+    <t>SOT-23-6</t>
+  </si>
+  <si>
+    <t>CL21B473KBCNNNC</t>
   </si>
 </sst>
 </file>
@@ -814,8 +817,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Label(s)" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type" dataDxfId="8"/>
@@ -1129,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,280 +1154,307 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" s="14">
-        <v>0.24</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4"/>
       <c r="D3" s="5" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="H3" s="5">
         <v>1</v>
       </c>
       <c r="I3" s="6">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="D4" s="5" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
       </c>
       <c r="I4" s="6">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5" s="6">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="H6" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="6">
-        <v>1.31</v>
+        <v>0.32</v>
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="E7" s="4"/>
       <c r="F7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H7" s="5">
-        <v>1</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.82</v>
       </c>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" t="s">
-        <v>42</v>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="5">
         <v>1</v>
       </c>
-      <c r="I8" s="8">
-        <v>1.45</v>
+      <c r="I8" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="5" t="s">
-        <v>45</v>
+      <c r="D9" t="s">
+        <v>25</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="8">
+        <v>1.45</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5">
         <v>2</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11">
-        <f>SUM(H2:H9)</f>
-        <v>9</v>
-      </c>
-      <c r="I10" s="12">
-        <f>SUM(I2:I9)</f>
-        <v>4.2200000000000006</v>
-      </c>
-      <c r="J10" s="11"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="I10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11">
+        <f>SUM(H2:H10)</f>
+        <v>13</v>
+      </c>
+      <c r="I11" s="12">
+        <f>SUM(I2:I10)</f>
+        <v>2.99</v>
+      </c>
+      <c r="J11" s="11"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -1486,20 +1516,20 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
@@ -1511,30 +1541,30 @@
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
@@ -1605,6 +1635,11 @@
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>